<commit_message>
Auto-committed on 2023/06/28 週三 11:33:17.49
</commit_message>
<xml_diff>
--- a/Program/Other/暫收款對帳-日調結表.xlsx
+++ b/Program/Other/暫收款對帳-日調結表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v06v2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72C9F39B-B9D3-4C7F-A591-9E8AF71A2FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1598BA55-DA4F-4648-9CE0-7D72857B8F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="804" yWindow="1464" windowWidth="22752" windowHeight="11628" xr2:uid="{565E1A71-423D-44C9-A149-405BD7F196AF}"/>
+    <workbookView xWindow="0" yWindow="612" windowWidth="22752" windowHeight="11628" xr2:uid="{565E1A71-423D-44C9-A149-405BD7F196AF}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +214,13 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -833,192 +840,195 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1334,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F49BE1-A9C5-4458-91E8-D27CB4A94DA6}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1357,173 +1367,180 @@
     <col min="14" max="14" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
-    <row r="2" spans="1:15" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:14" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="39" t="s">
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:14" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="9" t="s">
+      <c r="K3" s="28"/>
+      <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="28" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="25"/>
     </row>
-    <row r="5" spans="1:15" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="42"/>
+    <row r="5" spans="1:14" s="55" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
     </row>
-    <row r="6" spans="1:15" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="36" t="s">
+    <row r="6" spans="1:14" s="47" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="57"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62"/>
     </row>
-    <row r="7" spans="1:15" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="54" t="s">
+    <row r="7" spans="1:14" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:15" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="47" t="s">
+    <row r="9" spans="1:14" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="52"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:15" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
+    <row r="10" spans="1:14" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F2:F4"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
@@ -1533,12 +1550,6 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F2:F4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/06/28 週三 17:06:51.51
</commit_message>
<xml_diff>
--- a/Program/Other/暫收款對帳-日調結表.xlsx
+++ b/Program/Other/暫收款對帳-日調結表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v06v2\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1598BA55-DA4F-4648-9CE0-7D72857B8F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612C0599-F68D-4BDF-BD37-EDEE425B5BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="612" windowWidth="22752" windowHeight="11628" xr2:uid="{565E1A71-423D-44C9-A149-405BD7F196AF}"/>
+    <workbookView xWindow="288" yWindow="384" windowWidth="22752" windowHeight="11628" xr2:uid="{565E1A71-423D-44C9-A149-405BD7F196AF}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -652,19 +652,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thick">
         <color auto="1"/>
       </right>
@@ -830,6 +817,21 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -877,10 +879,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1">
@@ -892,34 +897,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -955,79 +1029,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1347,7 +1349,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1368,30 +1370,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:14" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="44" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="27" t="s">
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="51" t="s">
         <v>19</v>
       </c>
       <c r="L2" s="2"/>
@@ -1399,31 +1401,31 @@
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="34" t="s">
+      <c r="F3" s="42"/>
+      <c r="G3" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="28"/>
+      <c r="K3" s="52"/>
       <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1443,13 +1445,13 @@
       <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="29"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="53"/>
       <c r="L4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1460,42 +1462,42 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="55" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
+    <row r="5" spans="1:14" s="26" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
     </row>
-    <row r="6" spans="1:14" s="47" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="57"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
+    <row r="6" spans="1:14" s="18" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="60"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="62"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:14" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="20"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="14"/>
       <c r="I7" s="15"/>
     </row>
@@ -1503,11 +1505,11 @@
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="47"/>
       <c r="H8" s="16"/>
       <c r="I8" s="17"/>
     </row>
@@ -1515,11 +1517,11 @@
       <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
       <c r="H9" s="12"/>
       <c r="I9" s="13"/>
     </row>
@@ -1535,12 +1537,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F2:F4"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
@@ -1550,6 +1546,12 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F2:F4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/07/07 週五 11:42:50.52
</commit_message>
<xml_diff>
--- a/Program/Other/暫收款對帳-日調結表.xlsx
+++ b/Program/Other/暫收款對帳-日調結表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE68A41-BC1A-4E33-93A7-C00221464527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11928DF8-6728-45FD-9F45-B9138458F35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{565E1A71-423D-44C9-A149-405BD7F196AF}"/>
   </bookViews>
@@ -230,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -262,13 +262,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -308,17 +317,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F49BE1-A9C5-4458-91E8-D27CB4A94DA6}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -658,30 +673,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16" t="s">
         <v>19</v>
       </c>
       <c r="L2" s="2"/>
@@ -689,31 +704,31 @@
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="13"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
@@ -733,13 +748,13 @@
       <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="13"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="5" t="s">
         <v>15</v>
       </c>
@@ -751,45 +766,45 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
@@ -797,11 +812,11 @@
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
@@ -809,11 +824,11 @@
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
@@ -829,12 +844,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F2:F4"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
@@ -844,6 +853,12 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F2:F4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>